<commit_message>
Bowl analysis updates with finalized data and with new plotting scheme by order.
</commit_message>
<xml_diff>
--- a/WPP_Insect_Data_Summary.xlsx
+++ b/WPP_Insect_Data_Summary.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akrnz\Desktop\Analysis\WPP_Sample_Inventory_&amp;_Yield_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwolz/Desktop/RESEARCH/ACTIVE_PROJECTS/WPP_Biodiversity/WPP_Biodiversity_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
     <sheet name="aerial block order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="40">
   <si>
     <t>metric</t>
   </si>
@@ -142,13 +145,16 @@
   </si>
   <si>
     <t xml:space="preserve">ADAM </t>
+  </si>
+  <si>
+    <t>Alessa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -291,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -342,9 +348,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -679,47 +682,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AA63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21:Z22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="T22" sqref="T22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.875" style="1"/>
+    <col min="8" max="8" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1"/>
     <col min="11" max="11" width="6.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.125" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="11" style="8" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.875" style="1"/>
+    <col min="18" max="18" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" style="1"/>
     <col min="20" max="20" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="10.875" style="1"/>
+    <col min="27" max="27" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="16.5" thickBot="1">
+    <row r="1" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -796,7 +799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:27">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -873,7 +876,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -950,7 +953,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1027,7 +1030,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1181,7 +1184,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="16.5" thickBot="1">
+    <row r="7" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1412,7 +1415,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1566,7 +1569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1643,7 +1646,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="16.5" thickBot="1">
+    <row r="13" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>6</v>
       </c>
@@ -1720,7 +1723,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -1790,14 +1793,14 @@
       <c r="Y14" s="6">
         <v>1</v>
       </c>
-      <c r="Z14" s="4" t="s">
-        <v>12</v>
+      <c r="Z14" s="12" t="s">
+        <v>11</v>
       </c>
       <c r="AA14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
@@ -1874,7 +1877,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1947,14 +1950,14 @@
       <c r="Y16" s="6">
         <v>1</v>
       </c>
-      <c r="Z16" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA16" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27">
+      <c r="Z16" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA16" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -2024,14 +2027,14 @@
       <c r="Y17" s="6">
         <v>1</v>
       </c>
-      <c r="Z17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA17" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27">
+      <c r="Z17" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -2101,14 +2104,14 @@
       <c r="Y18" s="6">
         <v>1</v>
       </c>
-      <c r="Z18" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA18" s="19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" ht="16.5" thickBot="1">
+      <c r="Z18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA18" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>6</v>
       </c>
@@ -2181,14 +2184,14 @@
       <c r="Y19" s="7">
         <v>1</v>
       </c>
-      <c r="Z19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AA19" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
+      <c r="Z19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:27">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>6</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:27">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:27">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>6</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:27">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>6</v>
       </c>
@@ -2569,11 +2572,11 @@
       <c r="Z24" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AA24" s="19" t="s">
+      <c r="AA24" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="16.5" thickBot="1">
+    <row r="25" spans="1:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -2650,68 +2653,68 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:27">
-      <c r="K26" s="31" t="s">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="K26" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="31"/>
-      <c r="Q26" s="31"/>
-      <c r="R26" s="31"/>
-    </row>
-    <row r="27" spans="1:27">
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="32"/>
-    </row>
-    <row r="28" spans="1:27">
-      <c r="A28" s="33" t="s">
+      <c r="L26" s="30"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="1:27">
-      <c r="A29" s="34" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A29" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
-      <c r="F29" s="35"/>
-      <c r="G29" s="35"/>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35"/>
-    </row>
-    <row r="30" spans="1:27">
-      <c r="A30" s="34" t="s">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A30" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
-      <c r="H30" s="34"/>
-      <c r="I30" s="34"/>
-    </row>
-    <row r="32" spans="1:27">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2719,7 +2722,7 @@
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
     </row>
-    <row r="33" spans="11:16">
+    <row r="33" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2727,7 +2730,7 @@
       <c r="O33" s="1"/>
       <c r="P33" s="1"/>
     </row>
-    <row r="34" spans="11:16">
+    <row r="34" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2735,7 +2738,7 @@
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
     </row>
-    <row r="35" spans="11:16">
+    <row r="35" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2743,7 +2746,7 @@
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
     </row>
-    <row r="36" spans="11:16">
+    <row r="36" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
@@ -2751,7 +2754,7 @@
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="11:16">
+    <row r="37" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
@@ -2759,7 +2762,7 @@
       <c r="O37" s="1"/>
       <c r="P37" s="1"/>
     </row>
-    <row r="38" spans="11:16">
+    <row r="38" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2767,7 +2770,7 @@
       <c r="O38" s="1"/>
       <c r="P38" s="1"/>
     </row>
-    <row r="39" spans="11:16">
+    <row r="39" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2775,7 +2778,7 @@
       <c r="O39" s="1"/>
       <c r="P39" s="1"/>
     </row>
-    <row r="40" spans="11:16">
+    <row r="40" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
       <c r="M40" s="1"/>
@@ -2783,7 +2786,7 @@
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
     </row>
-    <row r="41" spans="11:16">
+    <row r="41" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
       <c r="M41" s="1"/>
@@ -2791,7 +2794,7 @@
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
     </row>
-    <row r="42" spans="11:16">
+    <row r="42" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
@@ -2799,7 +2802,7 @@
       <c r="O42" s="1"/>
       <c r="P42" s="1"/>
     </row>
-    <row r="43" spans="11:16">
+    <row r="43" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -2807,7 +2810,7 @@
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
     </row>
-    <row r="44" spans="11:16">
+    <row r="44" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
       <c r="M44" s="1"/>
@@ -2815,7 +2818,7 @@
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>
     </row>
-    <row r="45" spans="11:16">
+    <row r="45" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
@@ -2823,7 +2826,7 @@
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
     </row>
-    <row r="46" spans="11:16">
+    <row r="46" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
       <c r="M46" s="1"/>
@@ -2831,7 +2834,7 @@
       <c r="O46" s="1"/>
       <c r="P46" s="1"/>
     </row>
-    <row r="47" spans="11:16">
+    <row r="47" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
       <c r="M47" s="1"/>
@@ -2839,7 +2842,7 @@
       <c r="O47" s="1"/>
       <c r="P47" s="1"/>
     </row>
-    <row r="48" spans="11:16">
+    <row r="48" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -2847,7 +2850,7 @@
       <c r="O48" s="1"/>
       <c r="P48" s="1"/>
     </row>
-    <row r="49" spans="11:16">
+    <row r="49" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
@@ -2855,7 +2858,7 @@
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
     </row>
-    <row r="50" spans="11:16">
+    <row r="50" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
@@ -2863,7 +2866,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="11:16">
+    <row r="51" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2871,7 +2874,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="11:16">
+    <row r="52" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
       <c r="M52" s="1"/>
@@ -2879,7 +2882,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="11:16">
+    <row r="53" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1"/>
@@ -2887,7 +2890,7 @@
       <c r="O53" s="1"/>
       <c r="P53" s="1"/>
     </row>
-    <row r="54" spans="11:16">
+    <row r="54" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
@@ -2895,7 +2898,7 @@
       <c r="O54" s="1"/>
       <c r="P54" s="1"/>
     </row>
-    <row r="55" spans="11:16">
+    <row r="55" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
       <c r="M55" s="1"/>
@@ -2903,7 +2906,7 @@
       <c r="O55" s="1"/>
       <c r="P55" s="1"/>
     </row>
-    <row r="56" spans="11:16">
+    <row r="56" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
@@ -2911,7 +2914,7 @@
       <c r="O56" s="1"/>
       <c r="P56" s="1"/>
     </row>
-    <row r="57" spans="11:16">
+    <row r="57" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
@@ -2919,7 +2922,7 @@
       <c r="O57" s="1"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="11:16">
+    <row r="58" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
@@ -2927,7 +2930,7 @@
       <c r="O58" s="1"/>
       <c r="P58" s="1"/>
     </row>
-    <row r="59" spans="11:16">
+    <row r="59" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
       <c r="M59" s="1"/>
@@ -2935,7 +2938,7 @@
       <c r="O59" s="1"/>
       <c r="P59" s="1"/>
     </row>
-    <row r="60" spans="11:16">
+    <row r="60" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
@@ -2943,7 +2946,7 @@
       <c r="O60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="11:16">
+    <row r="61" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
       <c r="M61" s="1"/>
@@ -2951,7 +2954,7 @@
       <c r="O61" s="1"/>
       <c r="P61" s="1"/>
     </row>
-    <row r="62" spans="11:16">
+    <row r="62" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
@@ -2959,7 +2962,7 @@
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
     </row>
-    <row r="63" spans="11:16">
+    <row r="63" spans="11:16" x14ac:dyDescent="0.2">
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -2988,840 +2991,840 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="26.25">
-      <c r="A1" s="36">
+    <row r="1" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="35">
         <v>2014</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="E1" s="36">
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="E1" s="35">
         <v>2015</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="I1" s="36">
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="I1" s="35">
         <v>2016</v>
       </c>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-    </row>
-    <row r="2" spans="1:11" ht="26.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="E2" s="20" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="E2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="26.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="E3" s="22">
-        <v>1</v>
-      </c>
-      <c r="F3" s="23" t="s">
+    <row r="3" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="E3" s="21">
+        <v>1</v>
+      </c>
+      <c r="F3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="22">
-        <v>1</v>
-      </c>
-      <c r="J3" s="23" t="s">
+      <c r="I3" s="21">
+        <v>1</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="26.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="E4" s="22">
+    <row r="4" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="E4" s="21">
         <v>2</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="21">
         <v>2</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="23" t="s">
+      <c r="K4" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="E5" s="22">
+    <row r="5" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A5" s="27"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="E5" s="21">
         <v>3</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="23" t="s">
+      <c r="G5" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="21">
         <v>3</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="23" t="s">
+      <c r="K5" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="26.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="E6" s="22">
+    <row r="6" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A6" s="27"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="E6" s="21">
         <v>4</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="23" t="s">
+      <c r="G6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <v>4</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="26.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-    </row>
-    <row r="8" spans="1:11" ht="26.25">
-      <c r="A8" s="20" t="s">
+    <row r="7" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+    </row>
+    <row r="8" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="I8" s="20" t="s">
+      <c r="E8" s="25"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="I8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="J8" s="21" t="s">
+      <c r="J8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="K8" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="26.25">
-      <c r="A9" s="22">
-        <v>1</v>
-      </c>
-      <c r="B9" s="23" t="s">
+    <row r="9" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A9" s="21">
+        <v>1</v>
+      </c>
+      <c r="B9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="I9" s="22">
-        <v>1</v>
-      </c>
-      <c r="J9" s="23" t="s">
+      <c r="E9" s="27"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="I9" s="21">
+        <v>1</v>
+      </c>
+      <c r="J9" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="23" t="s">
+      <c r="K9" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="26.25">
-      <c r="A10" s="22">
+    <row r="10" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A10" s="21">
         <v>2</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="I10" s="22">
+      <c r="E10" s="27"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="I10" s="21">
         <v>2</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="26.25">
-      <c r="A11" s="22">
+    <row r="11" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A11" s="21">
         <v>3</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="I11" s="22">
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="I11" s="21">
         <v>3</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="26.25">
-      <c r="A12" s="22">
+    <row r="12" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A12" s="21">
         <v>4</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="I12" s="22">
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="I12" s="21">
         <v>4</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="26.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-    </row>
-    <row r="14" spans="1:11" ht="26.25">
-      <c r="A14" s="25" t="s">
+    <row r="13" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+    </row>
+    <row r="14" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="21" t="s">
+      <c r="C14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J14" s="21" t="s">
+      <c r="J14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="K14" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="26.25">
-      <c r="A15" s="22">
-        <v>1</v>
-      </c>
-      <c r="B15" s="23" t="s">
+    <row r="15" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A15" s="21">
+        <v>1</v>
+      </c>
+      <c r="B15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="22">
-        <v>1</v>
-      </c>
-      <c r="F15" s="23" t="s">
+      <c r="E15" s="21">
+        <v>1</v>
+      </c>
+      <c r="F15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="22">
-        <v>1</v>
-      </c>
-      <c r="J15" s="23" t="s">
+      <c r="I15" s="21">
+        <v>1</v>
+      </c>
+      <c r="J15" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="26.25">
-      <c r="A16" s="22">
+    <row r="16" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A16" s="21">
         <v>2</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="21">
         <v>2</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="21">
         <v>2</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="26.25">
-      <c r="A17" s="22">
+    <row r="17" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A17" s="21">
         <v>3</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="22">
+      <c r="E17" s="21">
         <v>3</v>
       </c>
-      <c r="F17" s="23" t="s">
+      <c r="F17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="23" t="s">
+      <c r="G17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="21">
         <v>3</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="23" t="s">
+      <c r="K17" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="26.25">
-      <c r="A18" s="22">
+    <row r="18" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A18" s="21">
         <v>4</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="22">
+      <c r="E18" s="21">
         <v>4</v>
       </c>
-      <c r="F18" s="23" t="s">
+      <c r="F18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I18" s="22">
+      <c r="I18" s="21">
         <v>4</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="26.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-    </row>
-    <row r="20" spans="1:11" ht="26.25">
-      <c r="A20" s="25" t="s">
+    <row r="19" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="21" t="s">
+      <c r="F20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I20" s="30"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" spans="1:11" ht="26.25">
-      <c r="A21" s="22">
-        <v>1</v>
-      </c>
-      <c r="B21" s="23" t="s">
+      <c r="I20" s="29"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+    </row>
+    <row r="21" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A21" s="21">
+        <v>1</v>
+      </c>
+      <c r="B21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="22">
-        <v>1</v>
-      </c>
-      <c r="F21" s="23" t="s">
+      <c r="E21" s="21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="23" t="s">
+      <c r="G21" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="28"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-    </row>
-    <row r="22" spans="1:11" ht="26.25">
-      <c r="A22" s="22">
+      <c r="I21" s="27"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+    </row>
+    <row r="22" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A22" s="21">
         <v>2</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="21">
         <v>2</v>
       </c>
-      <c r="F22" s="23" t="s">
+      <c r="F22" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="23" t="s">
+      <c r="G22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="28"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-    </row>
-    <row r="23" spans="1:11" ht="26.25">
-      <c r="A23" s="22">
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+    </row>
+    <row r="23" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A23" s="21">
         <v>3</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="22">
+      <c r="E23" s="21">
         <v>3</v>
       </c>
-      <c r="F23" s="23" t="s">
+      <c r="F23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="23" t="s">
+      <c r="G23" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-    </row>
-    <row r="24" spans="1:11" ht="26.25">
-      <c r="A24" s="22">
+      <c r="I23" s="27"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+    </row>
+    <row r="24" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A24" s="21">
         <v>4</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E24" s="22">
+      <c r="E24" s="21">
         <v>4</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="F24" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-    </row>
-    <row r="25" spans="1:11" ht="26.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-    </row>
-    <row r="26" spans="1:11" ht="26.25">
-      <c r="A26" s="25" t="s">
+      <c r="I24" s="27"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+    </row>
+    <row r="25" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="21" t="s">
+      <c r="F26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="21" t="s">
+      <c r="G26" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I26" s="25" t="s">
+      <c r="I26" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J26" s="21" t="s">
+      <c r="J26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="K26" s="21" t="s">
+      <c r="K26" s="20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="26.25">
-      <c r="A27" s="22">
-        <v>1</v>
-      </c>
-      <c r="B27" s="23" t="s">
+    <row r="27" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A27" s="21">
+        <v>1</v>
+      </c>
+      <c r="B27" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="22">
-        <v>1</v>
-      </c>
-      <c r="F27" s="23" t="s">
+      <c r="E27" s="21">
+        <v>1</v>
+      </c>
+      <c r="F27" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G27" s="23" t="s">
+      <c r="G27" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="22">
-        <v>1</v>
-      </c>
-      <c r="J27" s="23" t="s">
+      <c r="I27" s="21">
+        <v>1</v>
+      </c>
+      <c r="J27" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="K27" s="23" t="s">
+      <c r="K27" s="22" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="26.25">
-      <c r="A28" s="22">
+    <row r="28" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A28" s="21">
         <v>2</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="22">
+      <c r="E28" s="21">
         <v>2</v>
       </c>
-      <c r="F28" s="23" t="s">
+      <c r="F28" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="22">
+      <c r="I28" s="21">
         <v>2</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="K28" s="23" t="s">
+      <c r="K28" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="26.25">
-      <c r="A29" s="22">
+    <row r="29" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A29" s="21">
         <v>3</v>
       </c>
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E29" s="22">
+      <c r="E29" s="21">
         <v>3</v>
       </c>
-      <c r="F29" s="23" t="s">
+      <c r="F29" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G29" s="23" t="s">
+      <c r="G29" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I29" s="22">
+      <c r="I29" s="21">
         <v>3</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K29" s="23" t="s">
+      <c r="K29" s="22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="26.25">
-      <c r="A30" s="22">
+    <row r="30" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A30" s="21">
         <v>4</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="22">
+      <c r="E30" s="21">
         <v>4</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I30" s="22">
+      <c r="I30" s="21">
         <v>4</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K30" s="22" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="26.25">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-    </row>
-    <row r="32" spans="1:11" ht="26.25">
-      <c r="A32" s="25" t="s">
+    <row r="31" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+    </row>
+    <row r="32" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="E32" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="I32" s="30"/>
-      <c r="J32" s="27"/>
-      <c r="K32" s="27"/>
-    </row>
-    <row r="33" spans="1:11" ht="26.25">
-      <c r="A33" s="22">
-        <v>1</v>
-      </c>
-      <c r="B33" s="23" t="s">
+      <c r="I32" s="29"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="26"/>
+    </row>
+    <row r="33" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A33" s="21">
+        <v>1</v>
+      </c>
+      <c r="B33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="E33" s="22">
-        <v>1</v>
-      </c>
-      <c r="F33" s="23" t="s">
+      <c r="E33" s="21">
+        <v>1</v>
+      </c>
+      <c r="F33" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="23" t="s">
+      <c r="G33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="29"/>
-    </row>
-    <row r="34" spans="1:11" ht="26.25">
-      <c r="A34" s="22">
+      <c r="I33" s="27"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+    </row>
+    <row r="34" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A34" s="21">
         <v>2</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="E34" s="22">
+      <c r="E34" s="21">
         <v>2</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="23" t="s">
+      <c r="G34" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="28"/>
-      <c r="J34" s="29"/>
-      <c r="K34" s="29"/>
-    </row>
-    <row r="35" spans="1:11" ht="26.25">
-      <c r="A35" s="22">
+      <c r="I34" s="27"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A35" s="21">
         <v>3</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="22">
+      <c r="E35" s="21">
         <v>3</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="G35" s="23" t="s">
+      <c r="G35" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I35" s="28"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-    </row>
-    <row r="36" spans="1:11" ht="26.25">
-      <c r="A36" s="22">
+      <c r="I35" s="27"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+    </row>
+    <row r="36" spans="1:11" ht="26" x14ac:dyDescent="0.3">
+      <c r="A36" s="21">
         <v>4</v>
       </c>
-      <c r="B36" s="23" t="s">
+      <c r="B36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E36" s="22">
+      <c r="E36" s="21">
         <v>4</v>
       </c>
-      <c r="F36" s="23" t="s">
+      <c r="F36" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G36" s="23" t="s">
+      <c r="G36" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="I36" s="28"/>
-      <c r="J36" s="29"/>
-      <c r="K36" s="29"/>
+      <c r="I36" s="27"/>
+      <c r="J36" s="28"/>
+      <c r="K36" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>